<commit_message>
start using Manager.reset() create methods to check the input to DFBA and dynamic submodels
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_check_model_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_check_model_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="1460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-25240" yWindow="940" windowWidth="25000" windowHeight="15540" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="120">
   <si>
     <t>ID</t>
   </si>
@@ -95,12 +95,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>submodel_1</t>
-  </si>
-  <si>
-    <t>submodel_2</t>
-  </si>
-  <si>
     <t>specie_name_1</t>
   </si>
   <si>
@@ -396,6 +390,21 @@
   </si>
   <si>
     <t>U238</t>
+  </si>
+  <si>
+    <t>Min flux</t>
+  </si>
+  <si>
+    <t>Max flux</t>
+  </si>
+  <si>
+    <t>dfba_submodel</t>
+  </si>
+  <si>
+    <t>Objective proportion</t>
+  </si>
+  <si>
+    <t>ssa_submodel</t>
   </si>
 </sst>
 </file>
@@ -452,7 +461,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +472,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -484,7 +498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -497,8 +511,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -523,18 +539,23 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="9" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
   </cellStyles>
@@ -914,10 +935,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -925,23 +946,23 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -971,55 +992,55 @@
   <sheetData>
     <row r="1" spans="1:18" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>3</v>
@@ -1041,34 +1062,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1086,10 +1107,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1097,23 +1118,23 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1121,12 +1142,12 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1138,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1150,18 +1171,19 @@
     <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -1170,24 +1192,24 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
@@ -1195,16 +1217,16 @@
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -1232,22 +1254,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1258,13 +1280,13 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" s="6">
         <v>4.58E-17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1275,13 +1297,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="6">
         <v>9.9999999999999998E-13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1313,13 +1335,13 @@
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>8</v>
@@ -1340,21 +1362,21 @@
         <v>3</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1363,22 +1385,22 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -1387,22 +1409,22 @@
         <v>0</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -1411,23 +1433,23 @@
         <v>0</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1436,24 +1458,24 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1462,23 +1484,23 @@
         <v>0</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1487,18 +1509,18 @@
         <v>0</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F8" s="1">
         <v>10</v>
@@ -1507,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1568,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>14</v>
@@ -1555,12 +1577,12 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2">
         <v>1.4799999999999999E-4</v>
@@ -1568,7 +1590,7 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="2">
         <v>2.0000000000000001E-4</v>
@@ -1576,7 +1598,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2">
         <v>5.0000000000000001E-4</v>
@@ -1584,7 +1606,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="2">
         <v>5.0000000000000001E-4</v>
@@ -1592,7 +1614,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B6" s="2">
         <v>1E-3</v>
@@ -1600,7 +1622,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B7" s="2">
         <v>2E-3</v>
@@ -1617,9 +1639,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1627,12 +1651,16 @@
     <col min="2" max="2" width="24.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="8.83203125" style="1"/>
+    <col min="6" max="6" width="11.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1641,109 +1669,127 @@
         <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="7">
+        <v>87</v>
+      </c>
+      <c r="E2" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="9"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" s="7">
+        <v>88</v>
+      </c>
+      <c r="E3" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E4" s="7">
+        <v>89</v>
+      </c>
+      <c r="E4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>119</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E5" s="7">
+        <v>90</v>
+      </c>
+      <c r="E5" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="E6" s="7" t="b">
         <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1759,10 +1805,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1770,64 +1816,82 @@
     <col min="3" max="3" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="6">
         <v>2000</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D4" s="6">
         <v>2.9999999999999997E-4</v>
@@ -1835,16 +1899,22 @@
       <c r="E4" s="6">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
-      </c>
-      <c r="C5" t="s">
-        <v>105</v>
       </c>
       <c r="D5" s="6">
         <v>2.9999999999999997E-4</v>
@@ -1852,22 +1922,34 @@
       <c r="E5" s="6">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="6">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="E6" s="6">
         <v>1E-3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1894,16 +1976,16 @@
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>14</v>
@@ -1915,27 +1997,27 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" s="1">
         <v>0.3</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
portable NaN; update todos
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_check_model_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_check_model_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25240" yWindow="940" windowWidth="25000" windowHeight="15540" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="400" yWindow="2240" windowWidth="36140" windowHeight="15540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -1159,7 +1159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1641,8 +1641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1769,7 +1769,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1807,8 +1807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScale="189" zoomScaleNormal="189" zoomScalePageLayoutView="189" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adjust to move of flux bounds to reactions; check bounds & biomass reaction
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_check_model_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_check_model_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="400" yWindow="2240" windowWidth="36140" windowHeight="15540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="37480" windowHeight="21140" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -20,15 +20,17 @@
     <sheet name="Concentrations" sheetId="10" r:id="rId6"/>
     <sheet name="Reactions" sheetId="4" r:id="rId7"/>
     <sheet name="Rate laws" sheetId="11" r:id="rId8"/>
-    <sheet name="Parameters" sheetId="5" r:id="rId9"/>
-    <sheet name="References" sheetId="6" r:id="rId10"/>
-    <sheet name="Cross references" sheetId="12" r:id="rId11"/>
+    <sheet name="Biomass components" sheetId="15" r:id="rId9"/>
+    <sheet name="Biomass reactions" sheetId="16" r:id="rId10"/>
+    <sheet name="Parameters" sheetId="5" r:id="rId11"/>
+    <sheet name="References" sheetId="6" r:id="rId12"/>
+    <sheet name="Cross references" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Parameters!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">References!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">References!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!#REF!</definedName>
   </definedNames>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="129">
   <si>
     <t>ID</t>
   </si>
@@ -338,18 +340,6 @@
     <t>specie_4[c]</t>
   </si>
   <si>
-    <t>biomass</t>
-  </si>
-  <si>
-    <t>Metabolism production</t>
-  </si>
-  <si>
-    <t>metabolite</t>
-  </si>
-  <si>
-    <t>[c]: (2) specie_2 ==&gt; biomass</t>
-  </si>
-  <si>
     <t>backward</t>
   </si>
   <si>
@@ -401,10 +391,49 @@
     <t>dfba_submodel</t>
   </si>
   <si>
-    <t>Objective proportion</t>
-  </si>
-  <si>
     <t>ssa_submodel</t>
+  </si>
+  <si>
+    <t>Biomass reaction</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>biomass_id_001</t>
+  </si>
+  <si>
+    <t>biomass_comp_1</t>
+  </si>
+  <si>
+    <t>Metabolism_biomass</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>biomass_id_002</t>
+  </si>
+  <si>
+    <t>biomass_comp_2</t>
+  </si>
+  <si>
+    <t>biomass_id_003</t>
+  </si>
+  <si>
+    <t>biomass_comp_3</t>
+  </si>
+  <si>
+    <t>biomass_id_004</t>
+  </si>
+  <si>
+    <t>biomass_comp_4</t>
+  </si>
+  <si>
+    <t>Metabolism biomass reaction</t>
+  </si>
+  <si>
+    <t>No comment</t>
   </si>
 </sst>
 </file>
@@ -415,7 +444,7 @@
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -460,8 +489,31 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,6 +529,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -498,7 +556,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -513,8 +571,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -542,8 +601,19 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="14" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="14"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="14" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -558,6 +628,7 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9"/>
+    <cellStyle name="Normal 3" xfId="14"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -977,6 +1048,127 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="47.1640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1052,7 +1244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1200,7 +1392,7 @@
     </row>
     <row r="2" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>78</v>
@@ -1209,7 +1401,7 @@
         <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>4</v>
@@ -1217,7 +1409,7 @@
     </row>
     <row r="3" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>79</v>
@@ -1314,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1376,7 +1568,7 @@
         <v>75</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -1400,7 +1592,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -1424,7 +1616,7 @@
         <v>75</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
@@ -1449,7 +1641,7 @@
       </c>
       <c r="D5"/>
       <c r="E5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1475,7 +1667,7 @@
       </c>
       <c r="D6"/>
       <c r="E6" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F6">
         <v>5</v>
@@ -1500,7 +1692,7 @@
         <v>75</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -1510,26 +1702,6 @@
       </c>
       <c r="H7" s="2" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +1786,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2">
         <v>1E-3</v>
@@ -1622,7 +1794,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B7" s="2">
         <v>2E-3</v>
@@ -1639,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1652,13 +1824,13 @@
     <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="11.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="1"/>
+    <col min="6" max="7" width="10.83203125"/>
+    <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1674,17 +1846,20 @@
       <c r="E1" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1692,7 +1867,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>87</v>
@@ -1700,13 +1875,16 @@
       <c r="E2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="1">
+      <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1714,21 +1892,24 @@
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>88</v>
       </c>
       <c r="E3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="9"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1736,7 +1917,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>89</v>
@@ -1744,13 +1925,10 @@
       <c r="E4" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
@@ -1758,7 +1936,7 @@
         <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>90</v>
@@ -1766,31 +1944,8 @@
       <c r="E5" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D5">
@@ -1805,10 +1960,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="189" zoomScaleNormal="189" zoomScalePageLayoutView="189" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1816,7 +1971,7 @@
     <col min="3" max="3" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>46</v>
       </c>
@@ -1832,20 +1987,14 @@
       <c r="E1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -1853,16 +2002,10 @@
         <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -1870,20 +2013,14 @@
         <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="6">
         <v>2000</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1891,7 +2028,7 @@
         <v>85</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D4" s="6">
         <v>2.9999999999999997E-4</v>
@@ -1899,22 +2036,16 @@
       <c r="E4" s="6">
         <v>1E-3</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D5" s="6">
         <v>2.9999999999999997E-4</v>
@@ -1922,14 +2053,8 @@
       <c r="E5" s="6">
         <v>1E-3</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1944,12 +2069,6 @@
       </c>
       <c r="E6" s="6">
         <v>1E-3</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1959,69 +2078,120 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.1640625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="13.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="G1" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>94</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="14">
+        <v>-3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="14">
+        <v>-4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="14">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
make Submodel.objective_function optional - use biomass_function if not provided; update test models
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_check_model_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_check_model_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="37480" windowHeight="21140" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28020" windowHeight="17540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>No comment</t>
+  </si>
+  <si>
+    <t>Objective function</t>
+  </si>
+  <si>
+    <t>2*Metabolism_biomass</t>
   </si>
 </sst>
 </file>
@@ -1048,21 +1054,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="12"/>
+    <col min="3" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
@@ -1070,26 +1075,20 @@
         <v>1</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
         <v>119</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="12" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1349,10 +1348,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView zoomScale="217" zoomScaleNormal="217" zoomScalePageLayoutView="217" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1361,13 +1360,14 @@
     <col min="2" max="2" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="1"/>
+    <col min="5" max="6" width="12.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>34</v>
       </c>
@@ -1381,16 +1381,22 @@
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
@@ -1403,11 +1409,17 @@
       <c r="D2" t="s">
         <v>104</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>119</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>114</v>
       </c>
@@ -1420,7 +1432,10 @@
       <c r="D3" t="s">
         <v>71</v>
       </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1813,7 +1828,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1824,7 +1839,6 @@
     <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="7" width="10.83203125"/>
     <col min="8" max="8" width="11.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8.83203125" style="1"/>

</xml_diff>